<commit_message>
added code to make plots per change in rotation size
</commit_message>
<xml_diff>
--- a/ana/Endpoint from last trial vs decay model.xlsx
+++ b/ana/Endpoint from last trial vs decay model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Jenn\Documents\Varied_Prop_Adaptation\ana\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2170EDF4-92AA-463E-8661-A0D4D5EC16ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C8CB4C-21F7-462D-9478-6920630102AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{46B10C3C-FA1D-42C1-ACC2-614FE8D0158F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{46B10C3C-FA1D-42C1-ACC2-614FE8D0158F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -397,7 +397,7 @@
   <dimension ref="A1:C108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G100" sqref="G100"/>
+      <selection activeCell="F101" sqref="F101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>